<commit_message>
Iteration 6 Thiện và Đức
</commit_message>
<xml_diff>
--- a/Test Automation - SE Bonus/List testcases.xlsx
+++ b/Test Automation - SE Bonus/List testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh Duc\Desktop\Test-Automation-SE-Bonus\Test Automation - SE Bonus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4938A3-C385-46B9-A4E2-56B01B110612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF63F24-634F-4DAD-A047-A8C926F77D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2904" windowWidth="17280" windowHeight="8964" xr2:uid="{0AC447B2-C3DC-4B22-A606-8C68F41017BB}"/>
+    <workbookView xWindow="2496" yWindow="840" windowWidth="17280" windowHeight="8964" xr2:uid="{0AC447B2-C3DC-4B22-A606-8C68F41017BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,13 +256,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCC4125"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,28 +328,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -351,6 +345,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAC8933-711E-4E8C-A788-FE99A2CFF5D6}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -699,673 +705,651 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5">
         <v>36</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="5">
         <v>38</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="5">
         <v>39</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="5">
         <v>41</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="5">
         <v>43</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="45" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="5">
         <v>44</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
     </row>
     <row r="46" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
     </row>
     <row r="47" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
     </row>
     <row r="48" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
     </row>
     <row r="49" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A49" s="5">
         <v>48</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
     </row>
     <row r="50" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="5">
         <v>49</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
     </row>
     <row r="51" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="5">
         <v>50</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-    </row>
-    <row r="52" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="5">
-        <v>51</v>
-      </c>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-    </row>
-    <row r="53" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="5">
-        <v>52</v>
-      </c>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Iteration 12 Đức Và Thiện
44 PASS 6 FAIL
</commit_message>
<xml_diff>
--- a/Test Automation - SE Bonus/List testcases.xlsx
+++ b/Test Automation - SE Bonus/List testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh Duc\Desktop\Test-Automation-SE-Bonus\Test Automation - SE Bonus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF63F24-634F-4DAD-A047-A8C926F77D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF99709-06D3-4037-8ECE-3EE365F5C50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2496" yWindow="840" windowWidth="17280" windowHeight="8964" xr2:uid="{0AC447B2-C3DC-4B22-A606-8C68F41017BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0AC447B2-C3DC-4B22-A606-8C68F41017BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>#</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Test Case</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Admin Login</t>
   </si>
   <si>
@@ -193,6 +190,12 @@
   </si>
   <si>
     <t>Admin Edit Cohort</t>
+  </si>
+  <si>
+    <t>Testcase Type</t>
+  </si>
+  <si>
+    <t>Security</t>
   </si>
 </sst>
 </file>
@@ -313,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -357,6 +360,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAC8933-711E-4E8C-A788-FE99A2CFF5D6}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -693,8 +705,8 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -706,9 +718,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -719,9 +733,9 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="C3" s="17"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -732,9 +746,9 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="C4" s="16"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
@@ -745,9 +759,9 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="C5" s="16"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -758,9 +772,9 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="16"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -771,9 +785,9 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="C7" s="16"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -784,9 +798,9 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="C8" s="16"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -797,9 +811,9 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="10"/>
+        <v>9</v>
+      </c>
+      <c r="C9" s="16"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -810,9 +824,9 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="16"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -823,9 +837,9 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="10"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="16"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -836,9 +850,9 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="13"/>
+        <v>12</v>
+      </c>
+      <c r="C12" s="18"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -849,9 +863,9 @@
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="16"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -862,9 +876,9 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="C14" s="16"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -875,9 +889,9 @@
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="C15" s="16"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -888,9 +902,9 @@
         <v>15</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="C16" s="16"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -901,9 +915,9 @@
         <v>16</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="C17" s="16"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -914,9 +928,9 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="10"/>
+        <v>18</v>
+      </c>
+      <c r="C18" s="16"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -927,9 +941,9 @@
         <v>18</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="C19" s="16"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -940,9 +954,9 @@
         <v>19</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="C20" s="16"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -953,9 +967,9 @@
         <v>20</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="C21" s="16"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -966,7 +980,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -979,7 +993,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -992,7 +1006,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1005,7 +1019,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1018,7 +1032,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1031,7 +1045,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1044,7 +1058,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1057,7 +1071,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1070,7 +1084,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1083,7 +1097,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1096,7 +1110,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -1109,7 +1123,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -1122,7 +1136,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -1135,7 +1149,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -1148,7 +1162,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -1161,7 +1175,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -1174,7 +1188,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -1187,7 +1201,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -1200,7 +1214,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -1213,7 +1227,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -1226,7 +1240,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
@@ -1239,7 +1253,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
@@ -1252,7 +1266,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
@@ -1265,7 +1279,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
@@ -1278,7 +1292,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
@@ -1291,7 +1305,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
@@ -1304,7 +1318,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
@@ -1317,7 +1331,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
@@ -1330,7 +1344,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
@@ -1343,7 +1357,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>

</xml_diff>

<commit_message>
Iteration 13 Đức và Thiện
44 PASS 6 FAIL
</commit_message>
<xml_diff>
--- a/Test Automation - SE Bonus/List testcases.xlsx
+++ b/Test Automation - SE Bonus/List testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh Duc\Desktop\Test-Automation-SE-Bonus\Test Automation - SE Bonus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF99709-06D3-4037-8ECE-3EE365F5C50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F443BBE0-E24A-40FE-9857-6153AF7559B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0AC447B2-C3DC-4B22-A606-8C68F41017BB}"/>
+    <workbookView xWindow="26112" yWindow="1332" windowWidth="17280" windowHeight="8964" xr2:uid="{0AC447B2-C3DC-4B22-A606-8C68F41017BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="61">
   <si>
     <t>#</t>
   </si>
@@ -196,13 +196,34 @@
   </si>
   <si>
     <t>Security</t>
+  </si>
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +248,13 @@
     <font>
       <sz val="16"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -324,9 +352,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -337,9 +362,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -352,22 +374,28 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -684,21 +712,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAC8933-711E-4E8C-A788-FE99A2CFF5D6}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D51" sqref="A1:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
-    <col min="2" max="2" width="44" style="4" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="44" style="3" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,662 +737,709 @@
       <c r="C1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="5">
+      <c r="D1" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5">
+      <c r="D2" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="5">
+      <c r="C3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="5">
+      <c r="C4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="5">
+      <c r="C5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="5">
+      <c r="C6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="5">
+      <c r="C7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="5">
+      <c r="C8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="5">
+      <c r="C9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="5">
+      <c r="C10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="5">
+      <c r="C11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="5">
+      <c r="C12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="5">
+      <c r="C13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="5">
+      <c r="C14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="5">
+      <c r="C15" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="5">
+      <c r="C16" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="5">
+      <c r="C17" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="5">
+      <c r="C18" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="5">
+      <c r="C19" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="5">
+      <c r="C20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="5">
+      <c r="C21" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="5">
+      <c r="C22" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="5">
+      <c r="C23" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="5">
+      <c r="C24" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="5">
+      <c r="C25" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="5">
+      <c r="C26" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="5">
+      <c r="C27" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="5">
+      <c r="C28" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="5">
+      <c r="C29" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="5">
+      <c r="C30" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="5">
+      <c r="C31" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="5">
+      <c r="C32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="5">
+      <c r="C33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="5">
+      <c r="C34" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="5">
+      <c r="C35" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="5">
+      <c r="C36" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="5">
+      <c r="C37" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="5">
+      <c r="C38" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="5">
+      <c r="C39" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="5">
+      <c r="C40" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="5">
+      <c r="C41" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="5">
+      <c r="C42" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-    </row>
-    <row r="44" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="5">
+      <c r="C43" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-    </row>
-    <row r="45" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="5">
+      <c r="C44" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-    </row>
-    <row r="46" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="5">
+      <c r="C45" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-    </row>
-    <row r="47" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="5">
+      <c r="C46" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-    </row>
-    <row r="48" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="5">
+      <c r="C47" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-    </row>
-    <row r="49" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="5">
+      <c r="C48" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-    </row>
-    <row r="50" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="5">
+      <c r="C49" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="4">
         <v>49</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-    </row>
-    <row r="51" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="5">
+      <c r="C50" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
+      <c r="C51" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>